<commit_message>
convertendo pra grayscale antes
</commit_message>
<xml_diff>
--- a/Pasta1.xlsx
+++ b/Pasta1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="6">
   <si>
     <t>colorido</t>
   </si>
@@ -41,10 +41,7 @@
     <t>real</t>
   </si>
   <si>
-    <t>fp</t>
-  </si>
-  <si>
-    <t>Fn</t>
+    <t>testgray</t>
   </si>
 </sst>
 </file>
@@ -371,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BV13"/>
+  <dimension ref="A1:BV14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,609 +1272,833 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="str">
-        <f>IF(B2=B4,"OK","NOK")</f>
-        <v>OK</v>
-      </c>
-      <c r="C6" t="str">
-        <f>IF(C2=C4,"OK","NOK")</f>
-        <v>OK</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" ref="D6:BO6" si="0">IF(D2=D4,"OK","NOK")</f>
-        <v>OK</v>
-      </c>
-      <c r="E6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="G6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="H6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="J6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="K6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="L6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="M6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="N6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="O6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="P6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="Q6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="R6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="S6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="T6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="U6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="V6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="W6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="X6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="Y6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="Z6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AA6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AB6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AC6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AD6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AE6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AF6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AG6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AH6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AI6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="AJ6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AK6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AL6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AM6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AN6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="AO6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="AP6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="AQ6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="AR6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="AS6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="AT6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AU6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AV6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="AW6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AX6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AY6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="AZ6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="BA6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="BB6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="BC6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="BD6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="BE6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="BF6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="BG6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="BH6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="BI6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="BJ6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="BK6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="BL6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="BM6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="BN6" t="str">
-        <f t="shared" si="0"/>
-        <v>NOK</v>
-      </c>
-      <c r="BO6" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-      <c r="BP6" t="str">
-        <f t="shared" ref="BP6:BV6" si="1">IF(BP2=BP4,"OK","NOK")</f>
-        <v>OK</v>
-      </c>
-      <c r="BQ6" t="str">
-        <f t="shared" si="1"/>
-        <v>OK</v>
-      </c>
-      <c r="BR6" t="str">
-        <f t="shared" si="1"/>
-        <v>OK</v>
-      </c>
-      <c r="BS6" t="str">
-        <f t="shared" si="1"/>
-        <v>OK</v>
-      </c>
-      <c r="BT6" t="str">
-        <f t="shared" si="1"/>
-        <v>OK</v>
-      </c>
-      <c r="BU6" t="str">
-        <f t="shared" si="1"/>
-        <v>NOK</v>
-      </c>
-      <c r="BV6" t="str">
-        <f t="shared" si="1"/>
-        <v>NOK</v>
+    <row r="5" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" t="s">
+        <v>3</v>
+      </c>
+      <c r="T5" t="s">
+        <v>2</v>
+      </c>
+      <c r="U5" t="s">
+        <v>2</v>
+      </c>
+      <c r="V5" t="s">
+        <v>3</v>
+      </c>
+      <c r="W5" t="s">
+        <v>3</v>
+      </c>
+      <c r="X5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BO5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BP5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BQ5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BR5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BS5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BT5" t="s">
+        <v>3</v>
+      </c>
+      <c r="BU5" t="s">
+        <v>2</v>
+      </c>
+      <c r="BV5" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f>COUNTIF(B6:BV6,"OK")/73</f>
-        <v>0.71232876712328763</v>
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="str">
+        <f>IF(B2=B4,"OK","NOK")</f>
+        <v>OK</v>
+      </c>
+      <c r="C7" t="str">
+        <f>IF(C2=C4,"OK","NOK")</f>
+        <v>OK</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" ref="D7:BO7" si="0">IF(D2=D4,"OK","NOK")</f>
+        <v>OK</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="R7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="S7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="T7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="U7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="V7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="W7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="X7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="Y7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="Z7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AA7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AB7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AC7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AD7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AE7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AF7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AG7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AH7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AI7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="AJ7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AK7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AL7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AM7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AN7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="AO7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="AP7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="AQ7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="AR7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="AS7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="AT7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AU7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AV7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="AW7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AX7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AY7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="AZ7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="BA7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="BB7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="BC7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="BD7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="BE7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="BF7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="BG7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="BH7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="BI7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="BJ7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="BK7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="BL7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="BM7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="BN7" t="str">
+        <f t="shared" si="0"/>
+        <v>NOK</v>
+      </c>
+      <c r="BO7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+      <c r="BP7" t="str">
+        <f t="shared" ref="BP7:BV7" si="1">IF(BP2=BP4,"OK","NOK")</f>
+        <v>OK</v>
+      </c>
+      <c r="BQ7" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+      <c r="BR7" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+      <c r="BS7" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+      <c r="BT7" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+      <c r="BU7" t="str">
+        <f t="shared" si="1"/>
+        <v>NOK</v>
+      </c>
+      <c r="BV7" t="str">
+        <f t="shared" si="1"/>
+        <v>NOK</v>
       </c>
     </row>
     <row r="8" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="str">
-        <f>IF(B3=B4,"OK","NOK")</f>
-        <v>OK</v>
-      </c>
-      <c r="C8" t="str">
-        <f t="shared" ref="C8:BN8" si="2">IF(C3=C4,"OK","NOK")</f>
-        <v>OK</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="E8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="G8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="H8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="I8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="J8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="K8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="L8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="M8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="N8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="O8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="P8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="Q8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="R8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="S8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="T8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="U8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="V8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="W8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="X8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="Y8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="Z8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="AA8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="AB8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="AC8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="AD8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="AE8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="AF8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="AG8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="AH8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="AI8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="AJ8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="AK8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="AL8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="AM8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="AN8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="AO8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="AP8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="AQ8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="AR8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="AS8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="AT8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="AU8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="AV8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="AW8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="AX8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="AY8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="AZ8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="BA8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="BB8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="BC8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="BD8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="BE8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="BF8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="BG8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="BH8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="BI8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="BJ8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="BK8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="BL8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="BM8" t="str">
-        <f t="shared" si="2"/>
-        <v>OK</v>
-      </c>
-      <c r="BN8" t="str">
-        <f t="shared" si="2"/>
-        <v>NOK</v>
-      </c>
-      <c r="BO8" t="str">
-        <f t="shared" ref="BO8:BV8" si="3">IF(BO3=BO4,"OK","NOK")</f>
-        <v>OK</v>
-      </c>
-      <c r="BP8" t="str">
-        <f t="shared" si="3"/>
-        <v>OK</v>
-      </c>
-      <c r="BQ8" t="str">
-        <f t="shared" si="3"/>
-        <v>OK</v>
-      </c>
-      <c r="BR8" t="str">
-        <f t="shared" si="3"/>
-        <v>OK</v>
-      </c>
-      <c r="BS8" t="str">
-        <f t="shared" si="3"/>
-        <v>OK</v>
-      </c>
-      <c r="BT8" t="str">
-        <f t="shared" si="3"/>
-        <v>OK</v>
-      </c>
-      <c r="BU8" t="str">
-        <f t="shared" si="3"/>
-        <v>NOK</v>
-      </c>
-      <c r="BV8" t="str">
-        <f t="shared" si="3"/>
-        <v>NOK</v>
+      <c r="A8">
+        <f>COUNTIF(B7:BV7,"OK")/73</f>
+        <v>0.71232876712328763</v>
       </c>
     </row>
     <row r="9" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f>COUNTIF(B8:BV8,"OK")/73</f>
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="str">
+        <f>IF(B3=B4,"OK","NOK")</f>
+        <v>OK</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" ref="C9:BN9" si="2">IF(C3=C4,"OK","NOK")</f>
+        <v>OK</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="R9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="S9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="T9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="U9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="V9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="W9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="X9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="Y9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="Z9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="AA9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="AB9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="AC9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="AD9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="AE9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="AF9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="AG9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="AH9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="AI9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="AJ9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="AK9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="AL9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="AM9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="AN9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="AO9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="AP9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="AQ9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="AR9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="AS9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="AT9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="AU9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="AV9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="AW9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="AX9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="AY9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="AZ9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="BA9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="BB9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="BC9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="BD9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="BE9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="BF9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="BG9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="BH9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="BI9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="BJ9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="BK9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="BL9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="BM9" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+      <c r="BN9" t="str">
+        <f t="shared" si="2"/>
+        <v>NOK</v>
+      </c>
+      <c r="BO9" t="str">
+        <f t="shared" ref="BO9:BV9" si="3">IF(BO3=BO4,"OK","NOK")</f>
+        <v>OK</v>
+      </c>
+      <c r="BP9" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="BQ9" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="BR9" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="BS9" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="BT9" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="BU9" t="str">
+        <f t="shared" si="3"/>
+        <v>NOK</v>
+      </c>
+      <c r="BV9" t="str">
+        <f t="shared" si="3"/>
+        <v>NOK</v>
+      </c>
+    </row>
+    <row r="10" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>COUNTIF(B9:BV9,"OK")/73</f>
         <v>0.65753424657534243</v>
       </c>
     </row>
@@ -1885,15 +2106,311 @@
       <c r="A11" t="s">
         <v>5</v>
       </c>
+      <c r="B11" t="str">
+        <f>IF(B5=B4,"OK","NOK")</f>
+        <v>OK</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" ref="C11:BN11" si="4">IF(C5=C4,"OK","NOK")</f>
+        <v>OK</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="R11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="S11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="T11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="U11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="V11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="W11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="X11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="Y11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="Z11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AA11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AB11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AC11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AD11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AE11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AF11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AG11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AH11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AI11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="AJ11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AK11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AL11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AM11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AN11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="AO11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="AP11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="AQ11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="AR11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="AS11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="AT11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AU11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AV11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="AW11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AX11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AY11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="AZ11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="BA11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="BB11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="BC11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="BD11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="BE11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="BF11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="BG11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="BH11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="BI11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="BJ11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="BK11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="BL11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="BM11" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+      <c r="BN11" t="str">
+        <f t="shared" si="4"/>
+        <v>NOK</v>
+      </c>
+      <c r="BO11" t="str">
+        <f t="shared" ref="BO11:BV11" si="5">IF(BO5=BO4,"OK","NOK")</f>
+        <v>NOK</v>
+      </c>
+      <c r="BP11" t="str">
+        <f t="shared" si="5"/>
+        <v>OK</v>
+      </c>
+      <c r="BQ11" t="str">
+        <f t="shared" si="5"/>
+        <v>OK</v>
+      </c>
+      <c r="BR11" t="str">
+        <f t="shared" si="5"/>
+        <v>OK</v>
+      </c>
+      <c r="BS11" t="str">
+        <f t="shared" si="5"/>
+        <v>OK</v>
+      </c>
+      <c r="BT11" t="str">
+        <f t="shared" si="5"/>
+        <v>OK</v>
+      </c>
+      <c r="BU11" t="str">
+        <f t="shared" si="5"/>
+        <v>NOK</v>
+      </c>
+      <c r="BV11" t="str">
+        <f t="shared" si="5"/>
+        <v>NOK</v>
+      </c>
     </row>
     <row r="12" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="BL12" s="1"/>
+      <c r="A12">
+        <f>COUNTIF(B11:BV11,"OK")/73</f>
+        <v>0.69863013698630139</v>
+      </c>
     </row>
     <row r="13" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="BT13" s="1"/>
+      <c r="BL13" s="1"/>
+    </row>
+    <row r="14" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="I14" s="1"/>
+      <c r="BT14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>